<commit_message>
finished phylo signal analyses
</commit_message>
<xml_diff>
--- a/output/phylo_signal/phy_table.xlsx
+++ b/output/phylo_signal/phy_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsinkifi-my.sharepoint.com/personal/rodriart_ad_helsinki_fi/Documents/R/BBS/bbs_across_taxa/output/phylo_signal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5F7A1AD-0AA4-4397-B478-B98B958CF73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{A5F7A1AD-0AA4-4397-B478-B98B958CF73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED190957-A20B-4EAA-A5FE-4557EE46AE4A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A2B32664-8FF1-4F74-99C3-EEEBE32E3CC2}"/>
   </bookViews>
@@ -171,8 +171,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -203,15 +204,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +531,7 @@
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:P19"/>
+      <selection activeCell="J3" sqref="J3:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,10 +543,11 @@
     <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.54296875" customWidth="1"/>
-    <col min="11" max="11" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
     <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -627,13 +630,13 @@
         <v>4</v>
       </c>
       <c r="N3" s="1">
-        <v>1.1760337744587901</v>
+        <v>1.62941832060485</v>
       </c>
       <c r="O3" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
+        <v>0.30819815486149499</v>
+      </c>
+      <c r="P3" s="4">
+        <v>4.4943820224719104</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
@@ -665,13 +668,13 @@
         <v>6</v>
       </c>
       <c r="N4" s="1">
-        <v>7.3556813974434403E-5</v>
+        <v>0.91851897706157204</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>50</v>
+        <v>0.33206173586286503</v>
+      </c>
+      <c r="P4" s="4">
+        <v>8.9887640449438209</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -703,13 +706,13 @@
         <v>6</v>
       </c>
       <c r="N5" s="1">
-        <v>0.65164475905743902</v>
+        <v>8.0309151666851805E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>5.2426997280125599E-3</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
+        <v>0.106385467691284</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -741,13 +744,13 @@
         <v>6</v>
       </c>
       <c r="N6" s="1">
-        <v>0.462821400360591</v>
+        <v>0.69665240390286398</v>
       </c>
       <c r="O6" s="1">
-        <v>7.2485017025130296E-3</v>
-      </c>
-      <c r="P6">
-        <v>50</v>
+        <v>3.8200569330907097E-2</v>
+      </c>
+      <c r="P6" s="4">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -765,13 +768,13 @@
         <v>4</v>
       </c>
       <c r="N7" s="1">
-        <v>1.66805049606888</v>
+        <v>0.377407239940525</v>
       </c>
       <c r="O7" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
+        <v>9.5130223427525903E-2</v>
+      </c>
+      <c r="P7" s="4">
+        <v>82.022471910112401</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>